<commit_message>
restructure how data files are processed using meta file info
</commit_message>
<xml_diff>
--- a/sassie-ecco_daily-avg_variables_table.xlsx
+++ b/sassie-ecco_daily-avg_variables_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948A1565-0082-254D-B3B8-E6246D58FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D810C09-B263-9F47-A0B2-7B90B8F8BCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34300" yWindow="-7560" windowWidth="34260" windowHeight="28300" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23720" windowHeight="20380" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,12 +585,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -605,17 +617,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,15 +951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
@@ -999,7 +1010,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>150</v>
       </c>
       <c r="D2" t="s">
@@ -1034,7 +1045,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>160</v>
       </c>
       <c r="D3" t="s">
@@ -1069,7 +1080,7 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="D4" t="s">
@@ -1104,7 +1115,7 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>162</v>
       </c>
       <c r="D5" t="s">
@@ -1132,38 +1143,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="J6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1209,7 +1220,7 @@
       <c r="B8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>169</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1244,7 +1255,7 @@
       <c r="B9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>170</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1272,213 +1283,213 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="H10" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="H11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>167</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="H13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
         <v>17</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
         <v>17</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="5" t="s">
+      <c r="H15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J15" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1489,7 +1500,7 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>126</v>
       </c>
       <c r="D16" t="s">
@@ -1524,7 +1535,7 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>127</v>
       </c>
       <c r="D17" t="s">
@@ -1559,7 +1570,7 @@
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>132</v>
       </c>
       <c r="D18" t="s">
@@ -1594,7 +1605,7 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>134</v>
       </c>
       <c r="D19" t="s">
@@ -1629,7 +1640,7 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D20" t="s">
@@ -1664,7 +1675,7 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>128</v>
       </c>
       <c r="D21" t="s">
@@ -1699,7 +1710,7 @@
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>129</v>
       </c>
       <c r="D22" t="s">
@@ -1734,7 +1745,7 @@
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>130</v>
       </c>
       <c r="D23" t="s">
@@ -1769,7 +1780,7 @@
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>131</v>
       </c>
       <c r="D24" t="s">
@@ -1804,7 +1815,7 @@
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>135</v>
       </c>
       <c r="D25" t="s">
@@ -1839,7 +1850,7 @@
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>136</v>
       </c>
       <c r="D26" t="s">
@@ -1874,7 +1885,7 @@
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>139</v>
       </c>
       <c r="D27" t="s">
@@ -1909,7 +1920,7 @@
       <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>137</v>
       </c>
       <c r="D28" t="s">
@@ -1944,7 +1955,7 @@
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>140</v>
       </c>
       <c r="D29" t="s">
@@ -1979,7 +1990,7 @@
       <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>138</v>
       </c>
       <c r="D30" t="s">
@@ -2014,7 +2025,7 @@
       <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D31" t="s">
@@ -2049,7 +2060,7 @@
       <c r="B32" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>142</v>
       </c>
       <c r="D32" t="s">
@@ -2084,7 +2095,7 @@
       <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>143</v>
       </c>
       <c r="D33" t="s">
@@ -2119,7 +2130,7 @@
       <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D34" t="s">
@@ -2154,7 +2165,7 @@
       <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>145</v>
       </c>
       <c r="D35" t="s">
@@ -2189,7 +2200,7 @@
       <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" t="s">
         <v>151</v>
       </c>
       <c r="D36" t="s">
@@ -2224,7 +2235,7 @@
       <c r="B37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>159</v>
       </c>
       <c r="D37" t="s">
@@ -2252,108 +2263,108 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="5">
         <v>3</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="5">
         <v>0</v>
       </c>
-      <c r="H38" t="s">
-        <v>101</v>
-      </c>
-      <c r="I38" t="s">
-        <v>94</v>
-      </c>
-      <c r="J38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K38" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="H38" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="5">
         <v>3</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="5">
         <v>1</v>
       </c>
-      <c r="H39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I39" t="s">
-        <v>94</v>
-      </c>
-      <c r="J39" t="s">
-        <v>96</v>
-      </c>
-      <c r="K39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="H39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="5">
         <v>3</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="5">
         <v>2</v>
       </c>
-      <c r="H40" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" t="s">
-        <v>94</v>
-      </c>
-      <c r="J40" t="s">
-        <v>96</v>
-      </c>
-      <c r="K40" t="s">
+      <c r="H40" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2364,7 +2375,7 @@
       <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>153</v>
       </c>
       <c r="D41" t="s">
@@ -2399,7 +2410,7 @@
       <c r="B42" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>154</v>
       </c>
       <c r="D42" t="s">
@@ -2434,7 +2445,7 @@
       <c r="B43" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" t="s">
         <v>152</v>
       </c>
       <c r="D43" t="s">
@@ -2469,7 +2480,7 @@
       <c r="B44" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>155</v>
       </c>
       <c r="D44" t="s">
@@ -2504,7 +2515,7 @@
       <c r="B45" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>156</v>
       </c>
       <c r="D45" t="s">
@@ -2539,7 +2550,7 @@
       <c r="B46" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>157</v>
       </c>
       <c r="D46" t="s">
@@ -2574,7 +2585,7 @@
       <c r="B47" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>158</v>
       </c>
       <c r="D47" t="s">
@@ -2609,7 +2620,7 @@
       <c r="B48" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" t="s">
         <v>105</v>
       </c>
       <c r="D48" t="s">
@@ -2644,7 +2655,7 @@
       <c r="B49" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" t="s">
         <v>106</v>
       </c>
       <c r="D49" t="s">
@@ -2679,7 +2690,7 @@
       <c r="B50" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" t="s">
         <v>109</v>
       </c>
       <c r="D50" t="s">
@@ -2714,7 +2725,7 @@
       <c r="B51" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" t="s">
         <v>110</v>
       </c>
       <c r="D51" t="s">
@@ -2749,7 +2760,7 @@
       <c r="B52" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" t="s">
         <v>113</v>
       </c>
       <c r="D52" t="s">
@@ -2784,7 +2795,7 @@
       <c r="B53" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" t="s">
         <v>114</v>
       </c>
       <c r="D53" t="s">
@@ -2819,7 +2830,7 @@
       <c r="B54" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" t="s">
         <v>107</v>
       </c>
       <c r="D54" t="s">
@@ -2854,7 +2865,7 @@
       <c r="B55" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" t="s">
         <v>108</v>
       </c>
       <c r="D55" t="s">
@@ -2889,7 +2900,7 @@
       <c r="B56" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" t="s">
         <v>111</v>
       </c>
       <c r="D56" t="s">
@@ -2924,7 +2935,7 @@
       <c r="B57" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" t="s">
         <v>112</v>
       </c>
       <c r="D57" t="s">
@@ -2952,283 +2963,283 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58">
+    <row r="58" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="4">
         <v>4</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="4">
         <v>0</v>
       </c>
-      <c r="H58" t="s">
-        <v>101</v>
-      </c>
-      <c r="I58" t="s">
+      <c r="H58" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J58" t="s">
-        <v>96</v>
-      </c>
-      <c r="K58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="J58" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="4">
         <v>4</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="4">
         <v>1</v>
       </c>
-      <c r="H59" t="s">
-        <v>101</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="H59" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J59" t="s">
-        <v>96</v>
-      </c>
-      <c r="K59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="J59" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="4">
         <v>4</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="4">
         <v>2</v>
       </c>
-      <c r="H60" t="s">
-        <v>101</v>
-      </c>
-      <c r="I60" t="s">
+      <c r="H60" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I60" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J60" t="s">
-        <v>96</v>
-      </c>
-      <c r="K60" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="J60" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="4">
         <v>4</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="4">
         <v>3</v>
       </c>
-      <c r="H61" t="s">
-        <v>101</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="H61" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J61" t="s">
-        <v>96</v>
-      </c>
-      <c r="K61" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="J61" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="5">
         <v>4</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="5">
         <v>0</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H62" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K62" t="s">
+      <c r="K62" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63">
+    <row r="63" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="5">
         <v>4</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="5">
         <v>1</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64">
+    <row r="64" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="5">
         <v>4</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="5">
         <v>2</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H64" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K64" t="s">
+      <c r="K64" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65">
+    <row r="65" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="5">
         <v>4</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="5">
         <v>3</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J65" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K65" t="s">
+      <c r="K65" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3239,7 +3250,7 @@
       <c r="B66" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" t="s">
         <v>164</v>
       </c>
       <c r="D66" t="s">
@@ -3274,7 +3285,7 @@
       <c r="B67" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" t="s">
         <v>165</v>
       </c>
       <c r="D67" t="s">
@@ -3309,7 +3320,7 @@
       <c r="B68" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>166</v>
       </c>
       <c r="D68" t="s">
@@ -3339,7 +3350,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K68" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}"/>
-  <conditionalFormatting sqref="A1:K3 A48:K67 A44:B47 D44:K47 A8:K12 A69:K1048576 A68:B68 D68:K68 A43:K43 A33:K33 A41:B42 D41:K42 A31:B32 D31:K32 A21:K26 A20:B20 D20:K20 A28:K28 A27:B27 D27:K27 A30:K30 A29:B29 D29:K29 A36:K40 A34:B35 D34:K35 A4:B7 D4:K7 A14:K19 A13:B13 D13:K13">
+  <conditionalFormatting sqref="A1:K3 A4:B7 D4:K7 A8:K12 A13:B13 D13:K13 A14:K19 A20:B20 D20:K20 A21:K26 A27:B27 D27:K27 A28:K28 A29:B29 D29:K29 A30:K30 A31:B32 D31:K32 A33:K33 A34:B35 D34:K35 A36:K40 A41:B42 D41:K42 A43:K43 A44:B47 D44:K47 A48:K67 A68:B68 D68:K68 A69:K1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>

</xml_diff>

<commit_message>
tested changes to v2 script on local machine
</commit_message>
<xml_diff>
--- a/sassie-ecco_daily-avg_variables_table.xlsx
+++ b/sassie-ecco_daily-avg_variables_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D810C09-B263-9F47-A0B2-7B90B8F8BCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC436CD-2CF2-BF4C-B105-37CB5509114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23720" windowHeight="20380" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34520" windowHeight="20380" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,6 +604,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -617,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -627,6 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,143 +3110,143 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
+    <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="5">
+      <c r="F62" s="7">
         <v>4</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="7">
         <v>0</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H62" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="J62" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K62" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="5">
+    <row r="63" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="7">
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F63" s="5">
+      <c r="F63" s="7">
         <v>4</v>
       </c>
-      <c r="G63" s="5">
+      <c r="G63" s="7">
         <v>1</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H63" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J63" s="5" t="s">
+      <c r="J63" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
+    <row r="64" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F64" s="7">
         <v>4</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G64" s="7">
         <v>2</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H64" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J64" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K64" s="5" t="s">
+      <c r="K64" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="5">
+    <row r="65" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="7">
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F65" s="7">
         <v>4</v>
       </c>
-      <c r="G65" s="5">
+      <c r="G65" s="7">
         <v>3</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H65" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J65" s="5" t="s">
+      <c r="J65" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="K65" s="5" t="s">
+      <c r="K65" s="7" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated inventory of missing datasets
</commit_message>
<xml_diff>
--- a/sassie-ecco_daily-avg_variables_table.xlsx
+++ b/sassie-ecco_daily-avg_variables_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mzahn/github/SASSIE_downscale_ecco_v5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC436CD-2CF2-BF4C-B105-37CB5509114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B1FE33-D8E9-B74D-9361-AE25DF7F9EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34520" windowHeight="20380" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
+    <workbookView xWindow="34620" yWindow="-3280" windowWidth="38820" windowHeight="27100" xr2:uid="{E4E239F0-85BC-1949-AD3A-4F3A4CE5C2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="179">
   <si>
     <t>n_dims</t>
   </si>
@@ -555,6 +555,27 @@
   </si>
   <si>
     <t>KPP boundary layer depth, bulk Ri criterion</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Turned off early</t>
+  </si>
+  <si>
+    <t>NON ZERO - turned off early</t>
+  </si>
+  <si>
+    <t>ZERO - turned off early</t>
+  </si>
+  <si>
+    <t>these datasets only had 101 gz files - more than half of the gz files are empty (46 bytes)</t>
+  </si>
+  <si>
+    <t>num_missing_days</t>
+  </si>
+  <si>
+    <t>corrupt gz: ocean_vel_day_mean.0015120000.tar.gz</t>
   </si>
 </sst>
 </file>
@@ -585,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -604,12 +625,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -623,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -632,8 +647,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,9 +987,11 @@
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1009,8 +1025,14 @@
       <c r="K1" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1044,8 +1066,11 @@
       <c r="K2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1079,148 +1104,166 @@
       <c r="K3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="L3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="L4" s="4">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="L5" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="J6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>3</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1254,183 +1297,204 @@
       <c r="K8" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="L8" s="5">
+        <v>1811</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>3</v>
       </c>
-      <c r="G9" s="5">
-        <v>2</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="J9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L9" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="10" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>101</v>
-      </c>
-      <c r="I10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" t="s">
-        <v>96</v>
-      </c>
-      <c r="K10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="H10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="H11" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
+      <c r="E12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" t="s">
-        <v>94</v>
-      </c>
-      <c r="J12" t="s">
-        <v>96</v>
-      </c>
-      <c r="K12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="4">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1464,8 +1528,11 @@
       <c r="K14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1499,8 +1566,11 @@
       <c r="K15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1534,8 +1604,11 @@
       <c r="K16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1569,8 +1642,11 @@
       <c r="K17" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1604,8 +1680,11 @@
       <c r="K18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1639,8 +1718,11 @@
       <c r="K19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1674,8 +1756,11 @@
       <c r="K20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1709,8 +1794,11 @@
       <c r="K21" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1744,8 +1832,11 @@
       <c r="K22" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1779,8 +1870,11 @@
       <c r="K23" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1814,8 +1908,11 @@
       <c r="K24" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1849,8 +1946,11 @@
       <c r="K25" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1884,8 +1984,11 @@
       <c r="K26" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1919,8 +2022,11 @@
       <c r="K27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1954,8 +2060,11 @@
       <c r="K28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1989,8 +2098,11 @@
       <c r="K29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2024,8 +2136,11 @@
       <c r="K30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2059,8 +2174,11 @@
       <c r="K31" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2094,8 +2212,11 @@
       <c r="K32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2129,8 +2250,11 @@
       <c r="K33" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2164,8 +2288,11 @@
       <c r="K34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2199,8 +2326,11 @@
       <c r="K35" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2234,8 +2364,11 @@
       <c r="K36" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2269,43 +2402,49 @@
       <c r="K37" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="L37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38">
         <v>3</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38">
         <v>0</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" t="s">
+        <v>94</v>
+      </c>
+      <c r="L38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2339,43 +2478,52 @@
       <c r="K39" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="L39" s="5">
+        <v>2119</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" t="s">
         <v>6</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40">
         <v>3</v>
       </c>
-      <c r="G40" s="5">
-        <v>2</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" t="s">
+        <v>94</v>
+      </c>
+      <c r="J40" t="s">
+        <v>96</v>
+      </c>
+      <c r="K40" t="s">
+        <v>94</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2409,8 +2557,11 @@
       <c r="K41" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2444,8 +2595,11 @@
       <c r="K42" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2479,8 +2633,11 @@
       <c r="K43" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2514,8 +2671,11 @@
       <c r="K44" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2549,8 +2709,11 @@
       <c r="K45" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2584,8 +2747,11 @@
       <c r="K46" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2619,78 +2785,87 @@
       <c r="K47" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="L47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
+      <c r="F48" s="4">
+        <v>2</v>
+      </c>
+      <c r="G48" s="4">
         <v>0</v>
       </c>
-      <c r="H48" t="s">
-        <v>101</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="H48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J48" t="s">
-        <v>96</v>
-      </c>
-      <c r="K48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="J48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L48" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F49">
-        <v>2</v>
-      </c>
-      <c r="G49">
+      <c r="F49" s="4">
+        <v>2</v>
+      </c>
+      <c r="G49" s="4">
         <v>1</v>
       </c>
-      <c r="H49" t="s">
-        <v>101</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="H49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I49" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J49" t="s">
-        <v>96</v>
-      </c>
-      <c r="K49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J49" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L49" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2724,8 +2899,11 @@
       <c r="K50" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2759,8 +2937,11 @@
       <c r="K51" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2794,8 +2975,11 @@
       <c r="K52" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2829,535 +3013,613 @@
       <c r="K53" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="L53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="4">
         <v>4</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="4">
         <v>0</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K54" t="s">
+      <c r="K54" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="L54" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="4">
         <v>4</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="4">
         <v>1</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K55" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="L55" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="4">
         <v>4</v>
       </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="G56" s="4">
+        <v>2</v>
+      </c>
+      <c r="H56" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K56" t="s">
+      <c r="K56" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="L56" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="4">
         <v>4</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="4">
         <v>3</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H57" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K57" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="L57" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="5">
         <v>4</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="5">
         <v>0</v>
       </c>
-      <c r="H58" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I58" s="4" t="s">
+      <c r="H58" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I58" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J58" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+      <c r="J58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L58" s="5">
+        <v>1912</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="5">
         <v>4</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="5">
         <v>1</v>
       </c>
-      <c r="H59" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I59" s="4" t="s">
+      <c r="H59" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J59" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
+      <c r="J59" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L59" s="5">
+        <v>1912</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" t="s">
         <v>117</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" t="s">
         <v>78</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="4">
+      <c r="F60">
         <v>4</v>
       </c>
-      <c r="G60" s="4">
-        <v>2</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I60" s="4" t="s">
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I60" t="s">
         <v>99</v>
       </c>
-      <c r="J60" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+      <c r="J60" t="s">
+        <v>96</v>
+      </c>
+      <c r="K60" t="s">
+        <v>94</v>
+      </c>
+      <c r="L60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" t="s">
         <v>78</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61">
         <v>4</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61">
         <v>3</v>
       </c>
-      <c r="H61" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I61" s="4" t="s">
+      <c r="H61" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" t="s">
         <v>99</v>
       </c>
-      <c r="J61" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
+      <c r="J61" t="s">
+        <v>96</v>
+      </c>
+      <c r="K61" t="s">
+        <v>94</v>
+      </c>
+      <c r="L61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="5">
         <v>4</v>
       </c>
-      <c r="G62" s="7">
+      <c r="G62" s="5">
         <v>0</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H62" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I62" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J62" s="7" t="s">
+      <c r="J62" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K62" s="7" t="s">
+      <c r="K62" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
+      <c r="L62" s="5">
+        <v>2133</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="5">
         <v>4</v>
       </c>
-      <c r="G63" s="7">
+      <c r="G63" s="5">
         <v>1</v>
       </c>
-      <c r="H63" s="7" t="s">
+      <c r="H63" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I63" s="7" t="s">
+      <c r="I63" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J63" s="7" t="s">
+      <c r="J63" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K63" s="7" t="s">
+      <c r="K63" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
+      <c r="L63" s="5">
+        <v>2133</v>
+      </c>
+      <c r="M63" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="5">
         <v>4</v>
       </c>
-      <c r="G64" s="7">
-        <v>2</v>
-      </c>
-      <c r="H64" s="7" t="s">
+      <c r="G64" s="5">
+        <v>2</v>
+      </c>
+      <c r="H64" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I64" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J64" s="7" t="s">
+      <c r="J64" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K64" s="7" t="s">
+      <c r="K64" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
+      <c r="L64" s="5">
+        <v>2133</v>
+      </c>
+      <c r="M64" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F65" s="5">
         <v>4</v>
       </c>
-      <c r="G65" s="7">
+      <c r="G65" s="5">
         <v>3</v>
       </c>
-      <c r="H65" s="7" t="s">
+      <c r="H65" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I65" s="7" t="s">
+      <c r="I65" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J65" s="7" t="s">
+      <c r="J65" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K65" s="7" t="s">
+      <c r="K65" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="L65" s="5">
+        <v>2133</v>
+      </c>
+      <c r="M65" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N65" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="4">
         <v>3</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="4">
         <v>0</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K66" t="s">
+      <c r="K66" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="L66" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="4">
         <v>3</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="4">
         <v>1</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J67" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="L67" s="4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="4">
         <v>3</v>
       </c>
-      <c r="G68">
-        <v>2</v>
-      </c>
-      <c r="H68" t="s">
-        <v>101</v>
-      </c>
-      <c r="I68" t="s">
+      <c r="G68" s="4">
+        <v>2</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I68" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="J68" t="s">
-        <v>96</v>
-      </c>
-      <c r="K68" t="s">
-        <v>94</v>
+      <c r="J68" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L68" s="4">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K68" xr:uid="{8DBAD622-170B-ED43-8388-3F6C8186C5D2}"/>
-  <conditionalFormatting sqref="A1:K3 A4:B7 D4:K7 A8:K12 A13:B13 D13:K13 A14:K19 A20:B20 D20:K20 A21:K26 A27:B27 D27:K27 A28:K28 A29:B29 D29:K29 A30:K30 A31:B32 D31:K32 A33:K33 A34:B35 D34:K35 A36:K40 A41:B42 D41:K42 A43:K43 A44:B47 D44:K47 A48:K67 A68:B68 D68:K68 A69:K1048576">
+  <conditionalFormatting sqref="M1 A1:L3 A4:B7 D4:L7 A8:L12 A13:B13 D13:L13 A14:L19 A20:B20 D20:L20 A21:L24 A25:K26 L25:L38 A27:B27 D27:K27 A28:K28 A29:B29 D29:K29 A30:K30 A31:B32 D31:K32 A33:K33 A34:B35 D34:K35 A36:K38 M39 A39:L40 A41:B42 D41:L42 A43:L43 A44:B47 D44:L47 A48:L67 A68:B68 D68:L68 A69:L1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NA"</formula>
     </cfRule>

</xml_diff>